<commit_message>
Update CoinChangeProblem - DynamicProgramming.xlsx
</commit_message>
<xml_diff>
--- a/20210602/CoinChangeProblem - DynamicProgramming.xlsx
+++ b/20210602/CoinChangeProblem - DynamicProgramming.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documentos\Escuelas\Modelo\2021 Feb-Jul DTS2 Algoritmos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programas\2021 Algoritmos\dts-2021-algoritmos\20210602\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C822BEE-1A77-4D1A-B5BD-F4CD78BBE2F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC9071F7-382B-47C2-9E14-AAB94C0BCE09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{06022E96-9135-445F-93CF-27E8273CA6F0}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" activeTab="1" xr2:uid="{06022E96-9135-445F-93CF-27E8273CA6F0}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="9">
   <si>
     <t>0 =&gt; 1</t>
   </si>
@@ -59,6 +60,9 @@
   <si>
     <t>(DENOMINACIONES)</t>
   </si>
+  <si>
+    <t>QTY</t>
+  </si>
 </sst>
 </file>
 
@@ -73,7 +77,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -92,6 +96,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -105,7 +115,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -115,6 +125,10 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -432,8 +446,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75ABDDFA-AE50-4A5A-8386-E4631B3EDD2E}">
   <dimension ref="A1:Q13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8:A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -732,4 +746,300 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA86C63F-C6C7-43B0-977B-49EC4E638809}">
+  <dimension ref="A1:R8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection sqref="A1:Q5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="5.28515625" customWidth="1"/>
+    <col min="2" max="17" width="6.42578125" customWidth="1"/>
+    <col min="18" max="25" width="7" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="1">
+        <v>0</v>
+      </c>
+      <c r="D1" s="1">
+        <v>1</v>
+      </c>
+      <c r="E1" s="1">
+        <v>2</v>
+      </c>
+      <c r="F1" s="1">
+        <v>3</v>
+      </c>
+      <c r="G1" s="1">
+        <v>4</v>
+      </c>
+      <c r="H1" s="1">
+        <v>5</v>
+      </c>
+      <c r="I1" s="1">
+        <v>6</v>
+      </c>
+      <c r="J1" s="1">
+        <v>7</v>
+      </c>
+      <c r="K1" s="1">
+        <v>8</v>
+      </c>
+      <c r="L1" s="1">
+        <v>9</v>
+      </c>
+      <c r="M1" s="1">
+        <v>10</v>
+      </c>
+      <c r="N1" s="1">
+        <v>11</v>
+      </c>
+      <c r="O1" s="1">
+        <v>12</v>
+      </c>
+      <c r="P1" s="1">
+        <v>13</v>
+      </c>
+      <c r="Q1" s="1">
+        <v>14</v>
+      </c>
+      <c r="R1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>5</v>
+      </c>
+      <c r="B2" s="1">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2" s="6">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>2</v>
+      </c>
+      <c r="F2">
+        <v>3</v>
+      </c>
+      <c r="G2">
+        <v>4</v>
+      </c>
+      <c r="H2">
+        <v>5</v>
+      </c>
+      <c r="I2">
+        <v>6</v>
+      </c>
+      <c r="J2">
+        <v>7</v>
+      </c>
+      <c r="K2">
+        <v>8</v>
+      </c>
+      <c r="L2">
+        <v>9</v>
+      </c>
+      <c r="M2">
+        <v>10</v>
+      </c>
+      <c r="N2">
+        <v>11</v>
+      </c>
+      <c r="O2">
+        <v>12</v>
+      </c>
+      <c r="P2">
+        <v>13</v>
+      </c>
+      <c r="Q2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1">
+        <v>3</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>2</v>
+      </c>
+      <c r="F3" s="6">
+        <v>1</v>
+      </c>
+      <c r="G3">
+        <v>2</v>
+      </c>
+      <c r="H3">
+        <v>3</v>
+      </c>
+      <c r="I3">
+        <v>2</v>
+      </c>
+      <c r="J3">
+        <v>3</v>
+      </c>
+      <c r="K3">
+        <v>4</v>
+      </c>
+      <c r="L3">
+        <v>3</v>
+      </c>
+      <c r="M3">
+        <v>4</v>
+      </c>
+      <c r="N3">
+        <v>5</v>
+      </c>
+      <c r="O3">
+        <v>4</v>
+      </c>
+      <c r="P3">
+        <v>5</v>
+      </c>
+      <c r="Q3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>0</v>
+      </c>
+      <c r="B4" s="1">
+        <v>7</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>2</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4">
+        <v>2</v>
+      </c>
+      <c r="H4">
+        <v>3</v>
+      </c>
+      <c r="I4">
+        <v>2</v>
+      </c>
+      <c r="J4" s="6">
+        <v>1</v>
+      </c>
+      <c r="K4">
+        <v>2</v>
+      </c>
+      <c r="L4">
+        <v>3</v>
+      </c>
+      <c r="M4">
+        <v>2</v>
+      </c>
+      <c r="N4">
+        <v>3</v>
+      </c>
+      <c r="O4">
+        <v>4</v>
+      </c>
+      <c r="P4">
+        <v>3</v>
+      </c>
+      <c r="Q4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>8</v>
+      </c>
+      <c r="B5" s="1">
+        <v>11</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>2</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="G5">
+        <v>2</v>
+      </c>
+      <c r="H5">
+        <v>3</v>
+      </c>
+      <c r="I5">
+        <v>2</v>
+      </c>
+      <c r="J5">
+        <v>1</v>
+      </c>
+      <c r="K5">
+        <v>2</v>
+      </c>
+      <c r="L5">
+        <v>3</v>
+      </c>
+      <c r="M5">
+        <v>2</v>
+      </c>
+      <c r="N5" s="6">
+        <v>1</v>
+      </c>
+      <c r="O5">
+        <v>2</v>
+      </c>
+      <c r="P5">
+        <v>3</v>
+      </c>
+      <c r="Q5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C8" s="7"/>
+      <c r="E8" s="4"/>
+      <c r="H8" s="4"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>